<commit_message>
Earnings update for LULU
</commit_message>
<xml_diff>
--- a/Mid Tier Luxury/CPRI_MODEL.xlsx
+++ b/Mid Tier Luxury/CPRI_MODEL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\Mid Tier Luxury\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D35E99D-F9C7-4EF4-ACF4-98A3770146B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C1D17A-8A45-40C4-8FC5-B3526C772875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="185">
   <si>
     <t>Price</t>
   </si>
@@ -681,6 +681,12 @@
   </si>
   <si>
     <t>Operating margin in high single digit range for Michael Kors</t>
+  </si>
+  <si>
+    <t>9.45x</t>
+  </si>
+  <si>
+    <t>Went Private</t>
   </si>
 </sst>
 </file>
@@ -691,13 +697,19 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -801,6 +813,21 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -952,126 +979,139 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="13" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="14" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="7" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="14" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="14" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="12" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="13" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="13" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="6" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="15" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1411,7 +1451,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1442,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="13">
-        <v>16.989999999999998</v>
+        <v>21.2</v>
       </c>
       <c r="C4" s="14">
-        <v>45872</v>
+        <v>45903</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1455,8 +1495,8 @@
       <c r="B5" s="13">
         <v>118</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>4</v>
+      <c r="C5" s="104" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1465,7 +1505,7 @@
       </c>
       <c r="B6" s="13">
         <f xml:space="preserve"> B4 * B5</f>
-        <v>2004.8199999999997</v>
+        <v>2501.6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1496,7 +1536,7 @@
       </c>
       <c r="B9" s="13">
         <f>B6 - B7 + B8</f>
-        <v>4938.82</v>
+        <v>5435.6</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>28</v>
@@ -1515,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
   <dimension ref="A1:AX89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+    <sheetView topLeftCell="E13" workbookViewId="0">
       <selection activeCell="AB53" sqref="AB53"/>
     </sheetView>
   </sheetViews>
@@ -5981,8 +6021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD6AACC-FEA2-4C5B-AF79-59D39A66A975}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6055,7 +6095,7 @@
         <v>173</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>176</v>
@@ -6198,37 +6238,39 @@
       <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="105" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="107">
         <v>0.434</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="106" t="s">
         <v>169</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="106" t="s">
         <v>171</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="106" t="s">
         <v>164</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="106" t="s">
         <v>172</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="K7" s="32"/>
+      <c r="K7" s="108" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6236,6 +6278,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341BEE4C9A91F44BB4A4EF8E0A71E02" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db93f7cdcc50be3ddb7642c8d50e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="878aac0c-df32-40a9-a231-d93e9c7b9b1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b63aaf3684aa43c37ed0cc1f5c2cf36e" ns3:_="">
     <xsd:import namespace="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -6379,15 +6430,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6395,6 +6437,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6408,14 +6458,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>